<commit_message>
Institute related content was updated
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\REQUIREMENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalith\Desktop\Development\2020 Project Class BIT\Student Project - 2020\prisonManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D25DB89C-BC02-41AF-ADDB-007239AD82E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +64,6 @@
     <t>Institutes</t>
   </si>
   <si>
-    <t>Types</t>
-  </si>
-  <si>
     <t>Closed Prisons</t>
   </si>
   <si>
@@ -646,12 +644,15 @@
   </si>
   <si>
     <t>institute id</t>
+  </si>
+  <si>
+    <t>Types (Prison)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1100,11 +1101,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,23 +1141,23 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1175,34 +1176,34 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" t="s">
         <v>122</v>
-      </c>
-      <c r="H13" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1213,10 +1214,10 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
         <v>124</v>
-      </c>
-      <c r="F15" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1234,500 +1235,500 @@
         <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B119" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B125" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1740,7 +1741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1754,162 +1755,162 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qualification controller was changed
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalith\Desktop\Development\2020 Project Class BIT\Student Project - 2020\prisonManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project 2021 final\prisonManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D25DB89C-BC02-41AF-ADDB-007239AD82E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,7 +651,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1101,11 +1100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">

</xml_diff>